<commit_message>
small changes to BDO for biosteam version compatibility; more work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Element</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Stream-biodiesel</t>
   </si>
   <si>
+    <t>Stream-natural gas</t>
+  </si>
+  <si>
     <t>biorefinery</t>
   </si>
   <si>
@@ -62,6 +65,9 @@
   </si>
   <si>
     <t>Price [USD/gal]</t>
+  </si>
+  <si>
+    <t>Price [USD/cf]</t>
   </si>
   <si>
     <t>Electricity price [USD/kWh]</t>
@@ -428,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,55 +481,55 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>-0.04951276951276952</v>
+        <v>0.7131006891006892</v>
       </c>
       <c r="D4">
-        <v>0.9359428199428199</v>
+        <v>0.9342515862515863</v>
       </c>
       <c r="E4">
-        <v>0.9386124146124147</v>
+        <v>0.936799944799945</v>
       </c>
       <c r="F4">
-        <v>-0.9989685509685512</v>
+        <v>-0.9982920862920862</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>0.05889052689052689</v>
+        <v>0.1518918078918079</v>
       </c>
       <c r="D5">
-        <v>-0.1001844281844282</v>
+        <v>-0.146010158010158</v>
       </c>
       <c r="E5">
-        <v>-0.1018840138840139</v>
+        <v>-0.1480611880611881</v>
       </c>
       <c r="F5">
-        <v>0.03273850473850474</v>
+        <v>0.07563126363126363</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>0.3694265494265495</v>
+        <v>0.5108561948561949</v>
       </c>
       <c r="D6">
-        <v>0.3927206607206608</v>
+        <v>0.3182191142191143</v>
       </c>
       <c r="E6">
-        <v>0.3855362055362056</v>
+        <v>0.3110450150450151</v>
       </c>
       <c r="F6">
-        <v>-0.02827698427698428</v>
+        <v>0.05582589182589183</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -531,19 +537,19 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>0.4374632214632215</v>
+        <v>0.04962794562794563</v>
       </c>
       <c r="D7">
-        <v>0.01654072054072054</v>
+        <v>0.01102199902199902</v>
       </c>
       <c r="E7">
-        <v>0.01653184053184053</v>
+        <v>0.0114997074997075</v>
       </c>
       <c r="F7">
-        <v>-0.01436497436497437</v>
+        <v>-0.02419136419136419</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -551,19 +557,19 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.1774570534570535</v>
+        <v>-0.03935556335556336</v>
       </c>
       <c r="D8">
-        <v>0.01154164754164754</v>
+        <v>-0.0145985545985546</v>
       </c>
       <c r="E8">
-        <v>0.01124681924681925</v>
+        <v>-0.0146004746004746</v>
       </c>
       <c r="F8">
-        <v>0.004647388647388648</v>
+        <v>0.01045190245190245</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -571,62 +577,82 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0.2632688872688873</v>
+        <v>0.4217814017814018</v>
       </c>
       <c r="D9">
-        <v>0.002630774630774631</v>
+        <v>0.04146192546192547</v>
       </c>
       <c r="E9">
-        <v>0.002863442863442864</v>
+        <v>0.04139508539508539</v>
       </c>
       <c r="F9">
-        <v>0.0006054846054846055</v>
+        <v>-0.03745396945396946</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0.2579230259230259</v>
+        <v>0.01131419931419931</v>
       </c>
       <c r="D10">
-        <v>-0.02554254154254154</v>
+        <v>0.0110957150957151</v>
       </c>
       <c r="E10">
-        <v>-0.02571069771069771</v>
+        <v>0.01071749871749872</v>
       </c>
       <c r="F10">
-        <v>0.03576988776988777</v>
+        <v>0.002768282768282768</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>-0.6711427551427552</v>
+        <v>0.006857574857574859</v>
       </c>
       <c r="D11">
-        <v>-0.02785459585459586</v>
+        <v>0.01432754632754633</v>
       </c>
       <c r="E11">
-        <v>-0.02807760407760408</v>
+        <v>0.01431777831777832</v>
       </c>
       <c r="F11">
-        <v>0.02972173772173773</v>
+        <v>-0.003403647403647404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>-0.04123574923574924</v>
+      </c>
+      <c r="D12">
+        <v>-0.03217422817422817</v>
+      </c>
+      <c r="E12">
+        <v>-0.03213940413940414</v>
+      </c>
+      <c r="F12">
+        <v>0.006139218139218139</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A10:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
further work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Element</t>
   </si>
@@ -28,24 +28,27 @@
     <t>MFPP [USD/ton]</t>
   </si>
   <si>
-    <t>Biodiesel production [gal/ton]</t>
-  </si>
-  <si>
-    <t>Ethanol production [gal/ton]</t>
-  </si>
-  <si>
-    <t>Electricity production [kWhr/ton]</t>
-  </si>
-  <si>
-    <t>Natural gas consumption [cf/ton]</t>
-  </si>
-  <si>
-    <t>Productivity [GGE/ton]</t>
+    <t>Biodiesel production [MMGal/yr]</t>
+  </si>
+  <si>
+    <t>Ethanol production [MMGal/yr]</t>
+  </si>
+  <si>
+    <t>Electricity production [MMWhr/yr]</t>
+  </si>
+  <si>
+    <t>Natural gas consumption [MMcf/yr]</t>
+  </si>
+  <si>
+    <t>Productivity [MMGGE/yr]</t>
   </si>
   <si>
     <t>TCI [10^6*USD]</t>
   </si>
   <si>
+    <t>Heat exchanger network error [%]</t>
+  </si>
+  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -64,21 +67,18 @@
     <t>biorefinery</t>
   </si>
   <si>
-    <t>Fermentation</t>
+    <t>Lipid content [dry wt. %]</t>
+  </si>
+  <si>
+    <t>Lipid retention [%]</t>
+  </si>
+  <si>
+    <t>Additional lipid extraction efficiency [%]</t>
   </si>
   <si>
     <t>Capacity [ton/hr]</t>
   </si>
   <si>
-    <t>Lipid content [dry wt. %]</t>
-  </si>
-  <si>
-    <t>Efficiency [%]</t>
-  </si>
-  <si>
-    <t>Lipid retention [%]</t>
-  </si>
-  <si>
     <t>Price [USD/gal]</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>IRR [%]</t>
-  </si>
-  <si>
-    <t>Solids loading [%]</t>
   </si>
 </sst>
 </file>
@@ -452,13 +449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +468,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -497,294 +495,301 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C4">
-        <v>0.4597017157017158</v>
+        <v>0.01243446846537874</v>
       </c>
       <c r="D4">
-        <v>0.005396309396309397</v>
+        <v>0.9656979317159171</v>
       </c>
       <c r="E4">
-        <v>0.007411819411819412</v>
+        <v>-0.9710174906486995</v>
       </c>
       <c r="F4">
-        <v>0.02746269946269946</v>
+        <v>0.8874372113054882</v>
       </c>
       <c r="H4">
-        <v>0.1044981564981565</v>
+        <v>0.2822626935945077</v>
       </c>
       <c r="I4">
-        <v>0.9948455268455269</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.7359404309416171</v>
+      </c>
+      <c r="J4">
+        <v>0.8128816605944312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C5">
-        <v>-0.03570545970545971</v>
+        <v>0.02509148922765957</v>
       </c>
       <c r="D5">
-        <v>0.9765082605082605</v>
+        <v>0.05113234697329388</v>
       </c>
       <c r="E5">
-        <v>-0.9987138027138028</v>
+        <v>0.002162529782501191</v>
       </c>
       <c r="F5">
-        <v>0.9952183072183074</v>
+        <v>0.02141216898448675</v>
       </c>
       <c r="H5">
-        <v>0.8597326277326278</v>
+        <v>0.05909610255584409</v>
       </c>
       <c r="I5">
-        <v>0.08320599520599521</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.0280392776335711</v>
+      </c>
+      <c r="J5">
+        <v>0.007775770778389963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C6">
-        <v>0.05738055338055339</v>
+        <v>0.04700840933633637</v>
       </c>
       <c r="D6">
-        <v>0.1483606603606604</v>
+        <v>0.07846696883467874</v>
       </c>
       <c r="E6">
-        <v>-0.0140995220995221</v>
+        <v>0.006183976087359043</v>
       </c>
       <c r="F6">
-        <v>-0.04252917052917052</v>
+        <v>-0.04582844180113766</v>
       </c>
       <c r="H6">
-        <v>0.1072073632073632</v>
+        <v>0.0131443425097737</v>
       </c>
       <c r="I6">
-        <v>0.04577926577926578</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>-0.03494218690168747</v>
+      </c>
+      <c r="J6">
+        <v>-0.00186048525922314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C7">
-        <v>-0.009752265752265753</v>
+        <v>0.08224410194576406</v>
       </c>
       <c r="D7">
-        <v>0.2083350883350883</v>
+        <v>0.1696790897951636</v>
       </c>
       <c r="E7">
-        <v>-0.0493984573984574</v>
+        <v>0.1878381166335246</v>
       </c>
       <c r="F7">
-        <v>0.1167738927738928</v>
+        <v>0.3346338050333522</v>
       </c>
       <c r="H7">
-        <v>0.4967283287283287</v>
+        <v>0.7480470345298813</v>
       </c>
       <c r="I7">
-        <v>0.04369080769080769</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0.651344777029791</v>
+      </c>
+      <c r="J7">
+        <v>-0.05503422352114372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C8">
-        <v>0.7572390612390613</v>
+        <v>0.6458100750804029</v>
       </c>
       <c r="D8">
-        <v>-0.04483794883794884</v>
+        <v>-9.880109195204365E-05</v>
       </c>
       <c r="E8">
-        <v>0.04252630252630253</v>
+        <v>-0.01255370450214818</v>
       </c>
       <c r="F8">
-        <v>-0.04472543672543673</v>
+        <v>-0.006136763861470554</v>
       </c>
       <c r="H8">
-        <v>-0.04314382314382315</v>
+        <v>-0.02582272029690881</v>
       </c>
       <c r="I8">
-        <v>0.0006233046233046233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>-0.01007252075490083</v>
+      </c>
+      <c r="J8">
+        <v>0.005903371006685095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9">
-        <v>0.2158805158805159</v>
+        <v>0.4012926813317072</v>
       </c>
       <c r="D9">
-        <v>0.05093357093357093</v>
+        <v>-0.008648459673938385</v>
       </c>
       <c r="E9">
-        <v>-0.05352565752565753</v>
+        <v>0.01109807113192284</v>
       </c>
       <c r="F9">
-        <v>0.04997899397899398</v>
+        <v>-0.004602154168086166</v>
       </c>
       <c r="H9">
-        <v>0.03795861795861796</v>
+        <v>0.007134161373366454</v>
       </c>
       <c r="I9">
-        <v>-0.003427659427659427</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>-0.00381772325670893</v>
+      </c>
+      <c r="J9">
+        <v>0.0004124588326765355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C10">
-        <v>0.01476739476739477</v>
+        <v>0.02957110303884412</v>
       </c>
       <c r="D10">
-        <v>0.0006385566385566386</v>
+        <v>0.004337107085484283</v>
       </c>
       <c r="E10">
-        <v>0.003117651117651118</v>
+        <v>-0.01196715311868612</v>
       </c>
       <c r="F10">
-        <v>-0.001177105177105177</v>
+        <v>0.005288213395528535</v>
       </c>
       <c r="H10">
-        <v>0.01034614634614635</v>
+        <v>-0.005754100742164029</v>
       </c>
       <c r="I10">
-        <v>0.02117866517866518</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>-0.008027295681091826</v>
+      </c>
+      <c r="J10">
+        <v>-0.005842889612239713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C11">
-        <v>0.1305628905628906</v>
+        <v>0.1943246190689847</v>
       </c>
       <c r="D11">
-        <v>-0.0243005163005163</v>
+        <v>0.0001026954281078171</v>
       </c>
       <c r="E11">
-        <v>0.01358683358683359</v>
+        <v>-0.001599571359982854</v>
       </c>
       <c r="F11">
-        <v>-0.01022804222804223</v>
+        <v>0.0001663083906523356</v>
       </c>
       <c r="H11">
-        <v>-0.02304279504279505</v>
+        <v>-0.004358397582335903</v>
       </c>
       <c r="I11">
-        <v>0.09574285174285176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0.002187953655518146</v>
+      </c>
+      <c r="J11">
+        <v>0.001440911530258935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C12">
-        <v>0.07859127059127059</v>
+        <v>0.2058898845875954</v>
       </c>
       <c r="D12">
-        <v>-0.0348916548916549</v>
+        <v>0.1628570201142808</v>
       </c>
       <c r="E12">
-        <v>0.0351949671949672</v>
+        <v>0.1141017462280698</v>
       </c>
       <c r="F12">
-        <v>-0.03743962943962944</v>
+        <v>0.2876288941291557</v>
       </c>
       <c r="H12">
-        <v>-0.02906664506664507</v>
+        <v>0.575809326232373</v>
       </c>
       <c r="I12">
-        <v>-0.05660633660633661</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.01952330132493205</v>
+      </c>
+      <c r="J12">
+        <v>0.0188931194838866</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C13">
-        <v>-0.2580323220323221</v>
+        <v>-0.46037575111903</v>
       </c>
       <c r="D13">
-        <v>-0.00120985320985321</v>
+        <v>0.01137455632698225</v>
       </c>
       <c r="E13">
-        <v>0.005321429321429321</v>
+        <v>-0.01509476546779062</v>
       </c>
       <c r="F13">
-        <v>-0.002868758868758869</v>
+        <v>0.005795905863836234</v>
       </c>
       <c r="H13">
-        <v>0.01178182778182778</v>
+        <v>-0.009326392117055684</v>
       </c>
       <c r="I13">
-        <v>-0.004049524049524049</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
-        <v>0.0006936726936726937</v>
-      </c>
-      <c r="D14">
-        <v>-0.004248160248160248</v>
-      </c>
-      <c r="E14">
-        <v>-0.005463377463377463</v>
-      </c>
-      <c r="F14">
-        <v>0.005083337083337084</v>
-      </c>
-      <c r="H14">
-        <v>-0.01305546105546106</v>
-      </c>
-      <c r="I14">
-        <v>-0.007314151314151315</v>
+        <v>0.009080876331235051</v>
+      </c>
+      <c r="J13">
+        <v>0.005744321992254426</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:J1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A11:A13"/>
   </mergeCells>

</xml_diff>

<commit_message>
fix pressure on sugarcane biorefinery stripping column; further work on lipidcane2g
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Element</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>TCI [10^6*USD]</t>
+  </si>
+  <si>
+    <t>Feedstock consumption [ton/yr]</t>
   </si>
   <si>
     <t>Heat exchanger network error [%]</t>
@@ -449,13 +452,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +472,9 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -498,298 +502,361 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4">
-        <v>-0.02039300982524563</v>
+        <v>-0.6692507312682818</v>
       </c>
       <c r="D4">
-        <v>0.9029070726768171</v>
+        <v>0.9455111377784444</v>
       </c>
       <c r="E4">
-        <v>-0.9732258306457664</v>
+        <v>-0.9746238655966399</v>
       </c>
       <c r="F4">
-        <v>0.8416905422635568</v>
+        <v>-0.7387399684992125</v>
+      </c>
+      <c r="G4">
+        <v>0.9717001008114807</v>
       </c>
       <c r="H4">
-        <v>0.1085607140178505</v>
+        <v>-0.9712562814070353</v>
       </c>
       <c r="I4">
-        <v>0.6205175129378234</v>
+        <v>0.8680792019800497</v>
       </c>
       <c r="J4">
-        <v>0.7601530038250958</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>-0.06124653116327909</v>
+      </c>
+      <c r="K4">
+        <v>0.8636015900397511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>0.1104372609315233</v>
+        <v>-0.04949223730593266</v>
       </c>
       <c r="D5">
-        <v>0.2149898747468687</v>
+        <v>0.06121503037575941</v>
       </c>
       <c r="E5">
-        <v>-0.04046801170029252</v>
+        <v>-0.04262056551413786</v>
       </c>
       <c r="F5">
-        <v>0.1897907447686192</v>
+        <v>-0.00648766219155479</v>
+      </c>
+      <c r="G5">
+        <v>0.05310671232785925</v>
       </c>
       <c r="H5">
-        <v>0.2767329183229582</v>
+        <v>-0.0487302182554564</v>
       </c>
       <c r="I5">
-        <v>0.1823130578264457</v>
+        <v>0.1414355358883972</v>
       </c>
       <c r="J5">
-        <v>0.1504582614565364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>0.1361659041476037</v>
+      </c>
+      <c r="K5">
+        <v>-0.003388584714617866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>0.1106262656566414</v>
+        <v>0.09575189379734496</v>
       </c>
       <c r="D6">
-        <v>0.337094427360684</v>
+        <v>0.2289492237305933</v>
       </c>
       <c r="E6">
-        <v>-0.01311032775819396</v>
+        <v>-0.01302932573314333</v>
       </c>
       <c r="F6">
-        <v>-0.1315667891697292</v>
+        <v>-0.1023730593264832</v>
+      </c>
+      <c r="G6">
+        <v>0.0746671101052974</v>
       </c>
       <c r="H6">
-        <v>0.05746793669841747</v>
+        <v>-0.02339908497712443</v>
       </c>
       <c r="I6">
-        <v>-0.1340403510087753</v>
+        <v>-0.005352133803345085</v>
       </c>
       <c r="J6">
-        <v>0.1284437110927774</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>-0.06355658891472288</v>
+      </c>
+      <c r="K6">
+        <v>0.257598439960999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>0.1360939023475587</v>
+        <v>0.2084497112427811</v>
       </c>
       <c r="D7">
-        <v>0.08491862296557415</v>
+        <v>0.07732843321083029</v>
       </c>
       <c r="E7">
-        <v>0.2463901597539939</v>
+        <v>0.2422320558013951</v>
       </c>
       <c r="F7">
-        <v>0.2850956273906848</v>
+        <v>0.098775969399235</v>
+      </c>
+      <c r="G7">
+        <v>-0.1894033808159956</v>
       </c>
       <c r="H7">
-        <v>0.7307012675316885</v>
+        <v>0.2846921173029326</v>
       </c>
       <c r="I7">
-        <v>0.6927743193579841</v>
+        <v>0.2273846846171155</v>
       </c>
       <c r="J7">
-        <v>-0.1410440261006525</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.7776224405610143</v>
+      </c>
+      <c r="K7">
+        <v>0.05440336008400212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>0.6631080777019427</v>
+        <v>0.404707117677942</v>
       </c>
       <c r="D8">
-        <v>0.0461921548038701</v>
+        <v>0.05014775369384235</v>
       </c>
       <c r="E8">
-        <v>-0.02728568214205356</v>
+        <v>-0.02640666016650417</v>
       </c>
       <c r="F8">
-        <v>0.06711617790444763</v>
+        <v>-0.02898822470561765</v>
+      </c>
+      <c r="G8">
+        <v>0.05632516182572641</v>
       </c>
       <c r="H8">
-        <v>0.04327608190204756</v>
+        <v>-0.02670366759168979</v>
       </c>
       <c r="I8">
-        <v>0.06610965274131855</v>
+        <v>0.08715967899197483</v>
       </c>
       <c r="J8">
-        <v>0.03392934823370585</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>0.02759318982974574</v>
+      </c>
+      <c r="K8">
+        <v>0.02388509712742819</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>0.4182374559363984</v>
+        <v>0.4829295732393311</v>
       </c>
       <c r="D9">
-        <v>-0.09282082052051303</v>
+        <v>-0.08734718367959199</v>
       </c>
       <c r="E9">
-        <v>0.07926798169954251</v>
+        <v>0.07976299407485186</v>
       </c>
       <c r="F9">
-        <v>-0.0819545488637216</v>
+        <v>0.07667141678541965</v>
+      </c>
+      <c r="G9">
+        <v>-0.1064590552522034</v>
       </c>
       <c r="H9">
-        <v>-0.02108602715067877</v>
+        <v>0.08326258156453914</v>
       </c>
       <c r="I9">
-        <v>-0.02833570839270982</v>
+        <v>-0.06393309832745819</v>
       </c>
       <c r="J9">
-        <v>-0.0726558163954099</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>-0.01898597464936624</v>
+      </c>
+      <c r="K9">
+        <v>-0.02834170854271357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>0.102977574439361</v>
+        <v>0.0346388659716493</v>
       </c>
       <c r="D10">
-        <v>-0.002338558463961599</v>
+        <v>0.01862296557413936</v>
       </c>
       <c r="E10">
-        <v>-0.04251406285157129</v>
+        <v>-0.04279906997674943</v>
       </c>
       <c r="F10">
-        <v>0.02496662416560414</v>
+        <v>0.01545938648466212</v>
+      </c>
+      <c r="G10">
+        <v>0.03014522538480182</v>
       </c>
       <c r="H10">
-        <v>0.01120978024450611</v>
+        <v>-0.03860196504912623</v>
       </c>
       <c r="I10">
-        <v>-0.006360159003975101</v>
+        <v>0.0005055126378159455</v>
       </c>
       <c r="J10">
-        <v>0.03134028350708768</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>-0.0102377559438986</v>
+      </c>
+      <c r="K10">
+        <v>0.02878271956798921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11">
-        <v>0.192606315157879</v>
+        <v>-0.02483162079051977</v>
       </c>
       <c r="D11">
-        <v>0.063841596039901</v>
+        <v>0.07964449111227782</v>
       </c>
       <c r="E11">
-        <v>-0.03549688742218556</v>
+        <v>-0.03649891247281183</v>
       </c>
       <c r="F11">
-        <v>0.07115577889447237</v>
+        <v>0.001512037800945024</v>
+      </c>
+      <c r="G11">
+        <v>0.06364587184619598</v>
       </c>
       <c r="H11">
-        <v>0.08450311257781445</v>
+        <v>-0.04004050101252531</v>
       </c>
       <c r="I11">
-        <v>0.1063811595289882</v>
+        <v>0.1291982299557489</v>
       </c>
       <c r="J11">
-        <v>0.00633015825395635</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>0.09863796594914874</v>
+      </c>
+      <c r="K11">
+        <v>0.04034200855021376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12">
-        <v>0.1868896722418061</v>
+        <v>0.1043786094652366</v>
       </c>
       <c r="D12">
-        <v>0.1116717917947949</v>
+        <v>0.1072541813545339</v>
       </c>
       <c r="E12">
-        <v>0.1335498387459687</v>
+        <v>0.1292282307057677</v>
       </c>
       <c r="F12">
-        <v>0.2536038400960025</v>
+        <v>0.05785344633615841</v>
+      </c>
+      <c r="G12">
+        <v>-0.003881881669681422</v>
       </c>
       <c r="H12">
-        <v>0.5272991824795621</v>
+        <v>0.05946898672466813</v>
       </c>
       <c r="I12">
-        <v>-0.06806570164254108</v>
+        <v>-0.06612465311632792</v>
       </c>
       <c r="J12">
-        <v>0.003169579239480987</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>0.5283537088427211</v>
+      </c>
+      <c r="K12">
+        <v>-0.02064501612540313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13">
-        <v>-0.3846066151653792</v>
+        <v>-0.2452381309532738</v>
       </c>
       <c r="D13">
-        <v>-0.001168529213230331</v>
+        <v>-0.000475511887797195</v>
       </c>
       <c r="E13">
-        <v>-0.008241206030150754</v>
+        <v>-0.008041701042526064</v>
       </c>
       <c r="F13">
-        <v>0.01636690917272932</v>
+        <v>-0.03633990849771244</v>
+      </c>
+      <c r="G13">
+        <v>0.01312861104015852</v>
       </c>
       <c r="H13">
-        <v>0.0086987174679367</v>
+        <v>-0.00301057526438161</v>
       </c>
       <c r="I13">
-        <v>0.05195979899497488</v>
+        <v>0.05337283432085803</v>
       </c>
       <c r="J13">
-        <v>-0.0214310357758944</v>
+        <v>0.004314107852696318</v>
+      </c>
+      <c r="K13">
+        <v>0.006396159903997601</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:K1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A11:A13"/>
   </mergeCells>

</xml_diff>